<commit_message>
Update MODELO 4.17 Integrado_mportaciones_mensual.xlsx
</commit_message>
<xml_diff>
--- a/Agricultura/MODELOS/MODELO 4.17 Integrado_mportaciones_mensual.xlsx
+++ b/Agricultura/MODELOS/MODELO 4.17 Integrado_mportaciones_mensual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\DATA INTELLIGENCE Dropbox\Diseño DATA's\Tablas Madre\Agricultura\MODELOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF4D17-7837-46E4-968D-0FCBBB38A661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02B256F-329E-42AD-AD79-96F93329710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{5402BD67-523E-46F2-97D3-E3B02C663DDC}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="681">
   <si>
     <t>2019/2020</t>
   </si>
@@ -2070,6 +2070,42 @@
   </si>
   <si>
     <t>https://analytics.zoho.com/open-view/2395394000012001487?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod-cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007436</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007471</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007557</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007641?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007750?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012007821?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012008429?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012008532?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012008671?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012009118?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012009237?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000012009383?ZOHO_CRITERIA=%22Traspuesta%204.17_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
   </si>
 </sst>
 </file>
@@ -8824,9 +8860,9 @@
   <dimension ref="B1:W120"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="11" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
+      <selection pane="bottomLeft" activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10113,7 +10149,9 @@
       <c r="R33" s="46">
         <v>1</v>
       </c>
-      <c r="S33" s="15"/>
+      <c r="S33" s="15" t="s">
+        <v>669</v>
+      </c>
       <c r="V33" t="s">
         <v>638</v>
       </c>
@@ -10164,7 +10202,9 @@
       <c r="R34" s="46">
         <v>1</v>
       </c>
-      <c r="S34" s="15"/>
+      <c r="S34" s="15" t="s">
+        <v>670</v>
+      </c>
       <c r="V34" t="s">
         <v>638</v>
       </c>
@@ -10215,7 +10255,9 @@
       <c r="R35" s="46">
         <v>1</v>
       </c>
-      <c r="S35" s="15"/>
+      <c r="S35" s="15" t="s">
+        <v>671</v>
+      </c>
       <c r="V35" t="s">
         <v>638</v>
       </c>
@@ -10266,7 +10308,9 @@
       <c r="R36" s="46">
         <v>7</v>
       </c>
-      <c r="S36" s="15"/>
+      <c r="S36" s="15" t="s">
+        <v>672</v>
+      </c>
       <c r="V36" t="s">
         <v>638</v>
       </c>
@@ -10317,7 +10361,9 @@
       <c r="R37" s="46">
         <v>7</v>
       </c>
-      <c r="S37" s="15"/>
+      <c r="S37" s="15" t="s">
+        <v>673</v>
+      </c>
       <c r="V37" t="s">
         <v>638</v>
       </c>
@@ -10368,7 +10414,9 @@
       <c r="R38" s="46">
         <v>7</v>
       </c>
-      <c r="S38" s="15"/>
+      <c r="S38" s="15" t="s">
+        <v>674</v>
+      </c>
       <c r="V38" t="s">
         <v>638</v>
       </c>
@@ -10419,7 +10467,9 @@
       <c r="R39" s="46">
         <v>7</v>
       </c>
-      <c r="S39" s="15"/>
+      <c r="S39" s="15" t="s">
+        <v>675</v>
+      </c>
       <c r="V39" t="s">
         <v>638</v>
       </c>
@@ -10470,7 +10520,9 @@
       <c r="R40" s="46">
         <v>7</v>
       </c>
-      <c r="S40" s="15"/>
+      <c r="S40" s="15" t="s">
+        <v>676</v>
+      </c>
       <c r="V40" t="s">
         <v>638</v>
       </c>
@@ -10521,7 +10573,9 @@
       <c r="R41" s="46">
         <v>7</v>
       </c>
-      <c r="S41" s="15"/>
+      <c r="S41" s="15" t="s">
+        <v>677</v>
+      </c>
       <c r="V41" t="s">
         <v>638</v>
       </c>
@@ -10572,7 +10626,9 @@
       <c r="R42" s="46">
         <v>7</v>
       </c>
-      <c r="S42" s="15"/>
+      <c r="S42" s="15" t="s">
+        <v>678</v>
+      </c>
       <c r="V42" t="s">
         <v>638</v>
       </c>
@@ -10623,7 +10679,9 @@
       <c r="R43" s="46">
         <v>7</v>
       </c>
-      <c r="S43" s="15"/>
+      <c r="S43" s="15" t="s">
+        <v>679</v>
+      </c>
       <c r="V43" t="s">
         <v>638</v>
       </c>
@@ -10674,7 +10732,9 @@
       <c r="R44" s="46">
         <v>7</v>
       </c>
-      <c r="S44" s="15"/>
+      <c r="S44" s="15" t="s">
+        <v>680</v>
+      </c>
       <c r="V44" t="s">
         <v>638</v>
       </c>
@@ -14238,17 +14298,18 @@
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="S23" r:id="rId1" xr:uid="{510F560B-13FB-42F6-852E-767539F79631}"/>
+    <hyperlink ref="S32" r:id="rId2" xr:uid="{51EC4B26-8833-45BF-89E0-02452A7872CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId5"/>
+        <x14:slicer r:id="rId6"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>